<commit_message>
Zavrseno punjenje tabela nedostajucim vrednostima, sada treba da se zapocne dopuna datasetova za nedostajuce godine i drzave
</commit_message>
<xml_diff>
--- a/Fill NaN values dataset.xlsx
+++ b/Fill NaN values dataset.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
   <si>
     <t xml:space="preserve">X Boost Regression (XBR)</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t xml:space="preserve">UN MIGRANT STOCK BY ORIGIN AND DESTINATION 2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ratovi se ne mogu predvidjati</t>
   </si>
   <si>
     <t xml:space="preserve">WARS FORMATTED</t>
@@ -110,11 +113,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -134,65 +138,17 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Lohit Devanagari"/>
+      <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF0000EE"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Lohit Devanagari"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -201,50 +157,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF58220"/>
-        <bgColor rgb="FFFF6600"/>
+        <bgColor rgb="FFF37B70"/>
       </patternFill>
     </fill>
     <fill>
@@ -256,7 +170,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFADD58A"/>
-        <bgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FF99CCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEF413D"/>
+        <bgColor rgb="FFF37B70"/>
       </patternFill>
     </fill>
     <fill>
@@ -266,27 +186,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -332,7 +237,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -356,38 +261,33 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -395,7 +295,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -403,7 +303,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -411,74 +315,97 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="10" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000EE"/>
+      <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFADD58A"/>
@@ -490,7 +417,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFF37B70"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -506,13 +433,13 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF59C5C7"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFF58220"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFEF413D"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
@@ -535,8 +462,8 @@
   </sheetPr>
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F43" activeCellId="0" sqref="F43"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -544,11 +471,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="70.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.3"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.72"/>
@@ -616,123 +543,123 @@
       <c r="C6" s="5" t="n">
         <v>800.6754</v>
       </c>
-      <c r="D6" s="4" t="n">
+      <c r="D6" s="5" t="n">
         <v>950.3666</v>
       </c>
-      <c r="E6" s="4" t="n">
+      <c r="E6" s="5" t="n">
         <v>1069.778</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4" t="n">
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5" t="n">
         <v>253.048</v>
       </c>
-      <c r="I6" s="5" t="n">
+      <c r="I6" s="6" t="n">
         <v>194.1651</v>
       </c>
-      <c r="J6" s="4" t="n">
+      <c r="J6" s="5" t="n">
         <v>252.7337</v>
       </c>
-      <c r="K6" s="4" t="n">
+      <c r="K6" s="5" t="n">
         <v>266.4589</v>
       </c>
-      <c r="L6" s="6"/>
+      <c r="L6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="8" t="n">
+      <c r="B7" s="9" t="n">
         <v>-0.1963</v>
       </c>
-      <c r="C7" s="9" t="n">
+      <c r="C7" s="10" t="n">
         <v>-0.3734</v>
       </c>
-      <c r="D7" s="8" t="n">
+      <c r="D7" s="10" t="n">
         <v>-0.1974</v>
       </c>
-      <c r="E7" s="8" t="n">
+      <c r="E7" s="10" t="n">
         <v>-0.3387</v>
       </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8" t="n">
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10" t="n">
         <v>0.6816</v>
       </c>
-      <c r="I7" s="8" t="n">
+      <c r="I7" s="11" t="n">
         <v>0.6669</v>
       </c>
-      <c r="J7" s="8" t="n">
+      <c r="J7" s="10" t="n">
         <v>0.6815</v>
       </c>
-      <c r="K7" s="9" t="n">
+      <c r="K7" s="10" t="n">
         <v>0.6665</v>
       </c>
-      <c r="L7" s="10"/>
+      <c r="L7" s="12"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="4" t="n">
+      <c r="B11" s="13" t="n">
         <v>252.4114</v>
       </c>
-      <c r="C11" s="5" t="n">
+      <c r="C11" s="14" t="n">
         <v>233.5514</v>
       </c>
-      <c r="D11" s="4" t="n">
+      <c r="D11" s="14" t="n">
         <v>248.3989</v>
       </c>
-      <c r="E11" s="4" t="n">
+      <c r="E11" s="14" t="n">
         <v>1734.8652</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4" t="n">
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14" t="n">
         <v>207.5235</v>
       </c>
-      <c r="I11" s="4" t="n">
+      <c r="I11" s="14" t="n">
         <v>210.867</v>
       </c>
-      <c r="J11" s="5" t="n">
+      <c r="J11" s="14" t="n">
         <v>205.325</v>
       </c>
-      <c r="K11" s="4" t="n">
+      <c r="K11" s="14" t="n">
         <v>1210.7391</v>
       </c>
-      <c r="L11" s="6"/>
+      <c r="L11" s="15"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="8" t="n">
+      <c r="B12" s="16" t="n">
         <v>0.225</v>
       </c>
-      <c r="C12" s="8" t="n">
+      <c r="C12" s="17" t="n">
         <v>0.1456</v>
       </c>
-      <c r="D12" s="8" t="n">
+      <c r="D12" s="17" t="n">
         <v>0.2212</v>
       </c>
-      <c r="E12" s="9" t="n">
+      <c r="E12" s="17" t="n">
         <v>-0.0501</v>
       </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8" t="n">
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17" t="n">
         <v>0.3628</v>
       </c>
-      <c r="I12" s="9" t="n">
+      <c r="I12" s="17" t="n">
         <v>0.2286</v>
       </c>
-      <c r="J12" s="8" t="n">
+      <c r="J12" s="17" t="n">
         <v>0.3563</v>
       </c>
-      <c r="K12" s="8" t="n">
+      <c r="K12" s="17" t="n">
         <v>0.2671</v>
       </c>
-      <c r="L12" s="10"/>
+      <c r="L12" s="18"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
@@ -741,126 +668,126 @@
       <c r="B16" s="4" t="n">
         <v>711.9993</v>
       </c>
-      <c r="C16" s="5" t="n">
+      <c r="C16" s="19" t="n">
         <v>593.2072</v>
       </c>
-      <c r="D16" s="4" t="n">
+      <c r="D16" s="5" t="n">
         <v>711.9993</v>
       </c>
-      <c r="E16" s="4" t="n">
+      <c r="E16" s="5" t="n">
         <v>953.7236</v>
       </c>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4" t="n">
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5" t="n">
         <v>250.8493</v>
       </c>
-      <c r="I16" s="5" t="n">
+      <c r="I16" s="6" t="n">
         <v>162.6384</v>
       </c>
-      <c r="J16" s="4" t="n">
+      <c r="J16" s="5" t="n">
         <v>250.8493</v>
       </c>
-      <c r="K16" s="4" t="n">
+      <c r="K16" s="5" t="n">
         <v>436.2339</v>
       </c>
-      <c r="L16" s="6"/>
+      <c r="L16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="8" t="n">
+      <c r="B17" s="20" t="n">
         <v>-0.1156</v>
       </c>
-      <c r="C17" s="9" t="n">
+      <c r="C17" s="10" t="n">
         <v>-0.3403</v>
       </c>
-      <c r="D17" s="8" t="n">
+      <c r="D17" s="10" t="n">
         <v>-0.1156</v>
       </c>
-      <c r="E17" s="8" t="n">
+      <c r="E17" s="10" t="n">
         <v>-0.2485</v>
       </c>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8" t="n">
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10" t="n">
         <v>0.6069</v>
       </c>
-      <c r="I17" s="8" t="n">
+      <c r="I17" s="11" t="n">
         <v>0.6325</v>
       </c>
-      <c r="J17" s="8" t="n">
+      <c r="J17" s="10" t="n">
         <v>0.6069</v>
       </c>
-      <c r="K17" s="9" t="n">
+      <c r="K17" s="10" t="n">
         <v>0.4288</v>
       </c>
-      <c r="L17" s="10"/>
+      <c r="L17" s="12"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="11" t="n">
+      <c r="B21" s="4" t="n">
         <v>1085819.732</v>
       </c>
-      <c r="C21" s="11" t="n">
+      <c r="C21" s="5" t="n">
         <v>1085819.732</v>
       </c>
-      <c r="D21" s="11" t="n">
+      <c r="D21" s="5" t="n">
         <v>1085819.73205</v>
       </c>
-      <c r="E21" s="11" t="n">
+      <c r="E21" s="5" t="n">
         <v>1085819.732</v>
       </c>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11" t="n">
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5" t="n">
         <v>112854.8942</v>
       </c>
-      <c r="I21" s="11" t="n">
+      <c r="I21" s="6" t="n">
         <v>112854.8942</v>
       </c>
-      <c r="J21" s="11" t="n">
+      <c r="J21" s="5" t="n">
         <v>112854.8942</v>
       </c>
-      <c r="K21" s="11" t="n">
+      <c r="K21" s="5" t="n">
         <v>112854.8942</v>
       </c>
-      <c r="L21" s="12"/>
+      <c r="L21" s="7"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="13" t="n">
+      <c r="B22" s="9" t="n">
         <v>-2.8946</v>
       </c>
-      <c r="C22" s="13" t="n">
+      <c r="C22" s="10" t="n">
         <v>-2.8947</v>
       </c>
-      <c r="D22" s="13" t="n">
+      <c r="D22" s="10" t="n">
         <v>-2.8946</v>
       </c>
-      <c r="E22" s="13" t="n">
+      <c r="E22" s="10" t="n">
         <v>-2.8946</v>
       </c>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13" t="n">
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10" t="n">
         <v>0.5952</v>
       </c>
-      <c r="I22" s="13" t="n">
+      <c r="I22" s="11" t="n">
         <v>0.5952</v>
       </c>
-      <c r="J22" s="13" t="n">
+      <c r="J22" s="10" t="n">
         <v>0.5952</v>
       </c>
-      <c r="K22" s="13" t="n">
+      <c r="K22" s="10" t="n">
         <v>0.5952</v>
       </c>
-      <c r="L22" s="14"/>
+      <c r="L22" s="12"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
@@ -869,62 +796,62 @@
       <c r="B26" s="4" t="n">
         <v>4.2175</v>
       </c>
-      <c r="C26" s="5" t="n">
+      <c r="C26" s="19" t="n">
         <v>4.2175</v>
       </c>
-      <c r="D26" s="4" t="n">
+      <c r="D26" s="5" t="n">
         <v>4.2175</v>
       </c>
-      <c r="E26" s="4" t="n">
+      <c r="E26" s="5" t="n">
         <v>4.2175</v>
       </c>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4" t="n">
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5" t="n">
         <v>0.9334</v>
       </c>
-      <c r="I26" s="5" t="n">
+      <c r="I26" s="6" t="n">
         <v>0.9334</v>
       </c>
-      <c r="J26" s="4" t="n">
+      <c r="J26" s="5" t="n">
         <v>0.9334</v>
       </c>
-      <c r="K26" s="4" t="n">
+      <c r="K26" s="5" t="n">
         <v>0.9334</v>
       </c>
-      <c r="L26" s="6"/>
+      <c r="L26" s="7"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B27" s="8" t="n">
+      <c r="B27" s="9" t="n">
         <v>-2.1855</v>
       </c>
-      <c r="C27" s="9" t="n">
+      <c r="C27" s="21" t="n">
         <v>-2.1856</v>
       </c>
-      <c r="D27" s="8" t="n">
+      <c r="D27" s="10" t="n">
         <v>-2.1855</v>
       </c>
-      <c r="E27" s="8" t="n">
+      <c r="E27" s="10" t="n">
         <v>-2.1855</v>
       </c>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8" t="n">
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10" t="n">
         <v>0.2949</v>
       </c>
-      <c r="I27" s="9" t="n">
+      <c r="I27" s="11" t="n">
         <v>0.2949</v>
       </c>
-      <c r="J27" s="8" t="n">
+      <c r="J27" s="10" t="n">
         <v>0.2949</v>
       </c>
-      <c r="K27" s="8" t="n">
+      <c r="K27" s="10" t="n">
         <v>0.2949</v>
       </c>
-      <c r="L27" s="10"/>
+      <c r="L27" s="12"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
@@ -933,62 +860,62 @@
       <c r="B31" s="4" t="n">
         <v>104.8095</v>
       </c>
-      <c r="C31" s="5" t="n">
+      <c r="C31" s="19" t="n">
         <v>104.8095</v>
       </c>
-      <c r="D31" s="4" t="n">
+      <c r="D31" s="5" t="n">
         <v>104.8095</v>
       </c>
-      <c r="E31" s="4" t="n">
+      <c r="E31" s="5" t="n">
         <v>104.8095</v>
       </c>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4" t="n">
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5" t="n">
         <v>51.8573</v>
       </c>
-      <c r="I31" s="5" t="n">
+      <c r="I31" s="6" t="n">
         <v>51.8574</v>
       </c>
-      <c r="J31" s="4" t="n">
+      <c r="J31" s="5" t="n">
         <v>51.8573</v>
       </c>
-      <c r="K31" s="4" t="n">
+      <c r="K31" s="5" t="n">
         <v>51.8573</v>
       </c>
-      <c r="L31" s="6"/>
+      <c r="L31" s="7"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B32" s="8" t="n">
+      <c r="B32" s="9" t="n">
         <v>0.1571</v>
       </c>
-      <c r="C32" s="9" t="n">
+      <c r="C32" s="21" t="n">
         <v>0.1571</v>
       </c>
-      <c r="D32" s="8" t="n">
+      <c r="D32" s="10" t="n">
         <v>0.1571</v>
       </c>
-      <c r="E32" s="8" t="n">
+      <c r="E32" s="10" t="n">
         <v>0.1571</v>
       </c>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8" t="n">
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10" t="n">
         <v>0.5829</v>
       </c>
-      <c r="I32" s="9" t="n">
+      <c r="I32" s="11" t="n">
         <v>0.5829</v>
       </c>
-      <c r="J32" s="8" t="n">
+      <c r="J32" s="10" t="n">
         <v>0.5829</v>
       </c>
-      <c r="K32" s="8" t="n">
+      <c r="K32" s="10" t="n">
         <v>0.5829</v>
       </c>
-      <c r="L32" s="10"/>
+      <c r="L32" s="12"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
@@ -997,446 +924,452 @@
       <c r="B36" s="4" t="n">
         <v>1.0184</v>
       </c>
-      <c r="C36" s="5" t="n">
+      <c r="C36" s="19" t="n">
         <v>1.0184</v>
       </c>
-      <c r="D36" s="4" t="n">
+      <c r="D36" s="5" t="n">
         <v>1.0184</v>
       </c>
-      <c r="E36" s="4" t="n">
+      <c r="E36" s="5" t="n">
         <v>1.0184</v>
       </c>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4" t="n">
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5" t="n">
         <v>0.5257</v>
       </c>
-      <c r="I36" s="5" t="n">
+      <c r="I36" s="6" t="n">
         <v>0.5257</v>
       </c>
-      <c r="J36" s="4" t="n">
+      <c r="J36" s="5" t="n">
         <v>0.5257</v>
       </c>
-      <c r="K36" s="4" t="n">
+      <c r="K36" s="5" t="n">
         <v>0.5257</v>
       </c>
-      <c r="L36" s="6"/>
+      <c r="L36" s="7"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B37" s="8" t="n">
+      <c r="B37" s="9" t="n">
         <v>-0.2979</v>
       </c>
-      <c r="C37" s="9" t="n">
+      <c r="C37" s="21" t="n">
         <v>-0.2979</v>
       </c>
-      <c r="D37" s="8" t="n">
+      <c r="D37" s="10" t="n">
         <v>-0.2979</v>
       </c>
-      <c r="E37" s="8" t="n">
+      <c r="E37" s="10" t="n">
         <v>-0.2979</v>
       </c>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8" t="n">
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10" t="n">
         <v>0.3299</v>
       </c>
-      <c r="I37" s="9" t="n">
+      <c r="I37" s="11" t="n">
         <v>0.3299</v>
       </c>
-      <c r="J37" s="8" t="n">
+      <c r="J37" s="10" t="n">
         <v>0.3299</v>
       </c>
-      <c r="K37" s="8" t="n">
+      <c r="K37" s="10" t="n">
         <v>0.3299</v>
       </c>
-      <c r="L37" s="10"/>
+      <c r="L37" s="12"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B41" s="11" t="n">
+      <c r="B41" s="4" t="n">
         <v>2164570450737.76</v>
       </c>
-      <c r="C41" s="11" t="n">
+      <c r="C41" s="5" t="n">
         <v>2164570450737.76</v>
       </c>
-      <c r="D41" s="11" t="n">
+      <c r="D41" s="5" t="n">
         <v>2164570450737.76</v>
       </c>
-      <c r="E41" s="11" t="n">
+      <c r="E41" s="5" t="n">
         <v>2164570450737.76</v>
       </c>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11" t="n">
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5" t="n">
         <v>1047896278819.61</v>
       </c>
-      <c r="I41" s="11" t="n">
+      <c r="I41" s="6" t="n">
         <v>1047896278819.61</v>
       </c>
-      <c r="J41" s="11" t="n">
+      <c r="J41" s="5" t="n">
         <v>1047896278819.61</v>
       </c>
-      <c r="K41" s="11" t="n">
+      <c r="K41" s="5" t="n">
         <v>1047896278819.61</v>
       </c>
-      <c r="L41" s="12"/>
+      <c r="L41" s="7"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="7" t="s">
+      <c r="A42" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B42" s="13" t="n">
+      <c r="B42" s="9" t="n">
         <v>0.1674</v>
       </c>
-      <c r="C42" s="13" t="n">
+      <c r="C42" s="10" t="n">
         <v>0.1674</v>
       </c>
-      <c r="D42" s="13" t="n">
+      <c r="D42" s="10" t="n">
         <v>0.1674</v>
       </c>
-      <c r="E42" s="13" t="n">
+      <c r="E42" s="10" t="n">
         <v>0.1674</v>
       </c>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13" t="n">
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10" t="n">
         <v>0.5969</v>
       </c>
-      <c r="I42" s="13" t="n">
+      <c r="I42" s="11" t="n">
         <v>0.5969</v>
       </c>
-      <c r="J42" s="13" t="n">
+      <c r="J42" s="10" t="n">
         <v>0.5969</v>
       </c>
-      <c r="K42" s="13" t="n">
+      <c r="K42" s="10" t="n">
         <v>0.5969</v>
       </c>
-      <c r="L42" s="14"/>
+      <c r="L42" s="12"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="22"/>
+      <c r="F45" s="0" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B46" s="11" t="n">
+        <v>23</v>
+      </c>
+      <c r="B46" s="23" t="n">
         <v>0.2096</v>
       </c>
-      <c r="C46" s="11" t="n">
+      <c r="C46" s="24" t="n">
         <v>0.2096</v>
       </c>
-      <c r="D46" s="11" t="n">
+      <c r="D46" s="24" t="n">
         <v>0.2096</v>
       </c>
-      <c r="E46" s="11" t="n">
+      <c r="E46" s="24" t="n">
         <v>0.2096</v>
       </c>
-      <c r="F46" s="11"/>
-      <c r="G46" s="11"/>
-      <c r="H46" s="11" t="n">
+      <c r="F46" s="24"/>
+      <c r="G46" s="24"/>
+      <c r="H46" s="24" t="n">
         <v>0.2213</v>
       </c>
-      <c r="I46" s="11" t="n">
+      <c r="I46" s="24" t="n">
         <v>0.2213</v>
       </c>
-      <c r="J46" s="11" t="n">
+      <c r="J46" s="24" t="n">
         <v>0.2213</v>
       </c>
-      <c r="K46" s="11" t="n">
+      <c r="K46" s="24" t="n">
         <v>0.2213</v>
       </c>
-      <c r="L46" s="12"/>
+      <c r="L46" s="25"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B47" s="13" t="n">
+      <c r="A47" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B47" s="26" t="n">
         <v>0.1611</v>
       </c>
-      <c r="C47" s="13" t="n">
+      <c r="C47" s="27" t="n">
         <v>0.1611</v>
       </c>
-      <c r="D47" s="13" t="n">
+      <c r="D47" s="27" t="n">
         <v>0.1611</v>
       </c>
-      <c r="E47" s="13" t="n">
+      <c r="E47" s="27" t="n">
         <v>0.1611</v>
       </c>
-      <c r="F47" s="13"/>
-      <c r="G47" s="13"/>
-      <c r="H47" s="13" t="n">
+      <c r="F47" s="27"/>
+      <c r="G47" s="27"/>
+      <c r="H47" s="27" t="n">
         <v>0.1142</v>
       </c>
-      <c r="I47" s="13" t="n">
+      <c r="I47" s="27" t="n">
         <v>0.1142</v>
       </c>
-      <c r="J47" s="13" t="n">
+      <c r="J47" s="27" t="n">
         <v>0.1142</v>
       </c>
-      <c r="K47" s="13" t="n">
+      <c r="K47" s="27" t="n">
         <v>0.1142</v>
       </c>
-      <c r="L47" s="14"/>
+      <c r="L47" s="28"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B51" s="4" t="n">
         <v>0.0382</v>
       </c>
-      <c r="C51" s="5" t="n">
+      <c r="C51" s="19" t="n">
         <v>0.0358</v>
       </c>
-      <c r="D51" s="4" t="n">
+      <c r="D51" s="5" t="n">
         <v>0.0383</v>
       </c>
-      <c r="E51" s="4" t="n">
+      <c r="E51" s="5" t="n">
         <v>0.0383</v>
       </c>
-      <c r="F51" s="4"/>
-      <c r="G51" s="4"/>
-      <c r="H51" s="4" t="n">
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="6" t="n">
         <v>0.0103</v>
       </c>
-      <c r="I51" s="4" t="n">
+      <c r="I51" s="5" t="n">
         <v>0.011</v>
       </c>
-      <c r="J51" s="5" t="n">
+      <c r="J51" s="19" t="n">
         <v>0.0102</v>
       </c>
-      <c r="K51" s="4" t="n">
+      <c r="K51" s="5" t="n">
         <v>0.0142</v>
       </c>
-      <c r="L51" s="6"/>
+      <c r="L51" s="7"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B52" s="8" t="n">
+      <c r="A52" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B52" s="9" t="n">
         <v>0.611</v>
       </c>
-      <c r="C52" s="9" t="n">
+      <c r="C52" s="21" t="n">
         <v>0.6004</v>
       </c>
-      <c r="D52" s="8" t="n">
+      <c r="D52" s="10" t="n">
         <v>0.6103</v>
       </c>
-      <c r="E52" s="8" t="n">
+      <c r="E52" s="10" t="n">
         <v>0.6104</v>
       </c>
-      <c r="F52" s="8"/>
-      <c r="G52" s="8"/>
-      <c r="H52" s="8" t="n">
+      <c r="F52" s="10"/>
+      <c r="G52" s="10"/>
+      <c r="H52" s="11" t="n">
         <v>0.895</v>
       </c>
-      <c r="I52" s="8" t="n">
+      <c r="I52" s="10" t="n">
         <v>0.8773</v>
       </c>
-      <c r="J52" s="8" t="n">
+      <c r="J52" s="21" t="n">
         <v>0.8955</v>
       </c>
-      <c r="K52" s="9" t="n">
+      <c r="K52" s="10" t="n">
         <v>0.8556</v>
       </c>
-      <c r="L52" s="10"/>
+      <c r="L52" s="12"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B56" s="4" t="n">
         <v>0.0325</v>
       </c>
-      <c r="C56" s="5" t="n">
+      <c r="C56" s="19" t="n">
         <v>0.0295</v>
       </c>
-      <c r="D56" s="4" t="n">
+      <c r="D56" s="5" t="n">
         <v>0.0325</v>
       </c>
-      <c r="E56" s="4" t="n">
+      <c r="E56" s="5" t="n">
         <v>0.0319</v>
       </c>
-      <c r="F56" s="4"/>
-      <c r="G56" s="4"/>
-      <c r="H56" s="5" t="n">
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="6" t="n">
         <v>0.0078</v>
       </c>
-      <c r="I56" s="4" t="n">
+      <c r="I56" s="5" t="n">
         <v>0.0085</v>
       </c>
-      <c r="J56" s="4" t="n">
+      <c r="J56" s="5" t="n">
         <v>0.008</v>
       </c>
-      <c r="K56" s="4" t="n">
+      <c r="K56" s="5" t="n">
         <v>0.0111</v>
       </c>
-      <c r="L56" s="6"/>
+      <c r="L56" s="7"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B57" s="8" t="n">
+      <c r="A57" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B57" s="9" t="n">
         <v>0.6079</v>
       </c>
-      <c r="C57" s="9" t="n">
+      <c r="C57" s="21" t="n">
         <v>0.6</v>
       </c>
-      <c r="D57" s="8" t="n">
+      <c r="D57" s="10" t="n">
         <v>0.6079</v>
       </c>
-      <c r="E57" s="8" t="n">
+      <c r="E57" s="10" t="n">
         <v>0.6118</v>
       </c>
-      <c r="F57" s="8"/>
-      <c r="G57" s="8"/>
-      <c r="H57" s="8" t="n">
+      <c r="F57" s="10"/>
+      <c r="G57" s="10"/>
+      <c r="H57" s="11" t="n">
         <v>0.9054</v>
       </c>
-      <c r="I57" s="8" t="n">
+      <c r="I57" s="10" t="n">
         <v>0.8848</v>
       </c>
-      <c r="J57" s="8" t="n">
+      <c r="J57" s="10" t="n">
         <v>0.9025</v>
       </c>
-      <c r="K57" s="9" t="n">
+      <c r="K57" s="10" t="n">
         <v>0.8646</v>
       </c>
-      <c r="L57" s="10"/>
+      <c r="L57" s="12"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B61" s="4" t="n">
         <v>0.0295</v>
       </c>
-      <c r="C61" s="5" t="n">
+      <c r="C61" s="19" t="n">
         <v>0.0275</v>
       </c>
-      <c r="D61" s="4" t="n">
+      <c r="D61" s="5" t="n">
         <v>0.0295</v>
       </c>
-      <c r="E61" s="4" t="n">
+      <c r="E61" s="5" t="n">
         <v>0.0308</v>
       </c>
-      <c r="F61" s="4"/>
-      <c r="G61" s="4"/>
-      <c r="H61" s="5" t="n">
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+      <c r="H61" s="6" t="n">
         <v>0.0132</v>
       </c>
-      <c r="I61" s="4" t="n">
+      <c r="I61" s="5" t="n">
         <v>0.0138</v>
       </c>
-      <c r="J61" s="4" t="n">
+      <c r="J61" s="5" t="n">
         <v>0.0135</v>
       </c>
-      <c r="K61" s="4" t="n">
+      <c r="K61" s="5" t="n">
         <v>0.016</v>
       </c>
-      <c r="L61" s="6"/>
+      <c r="L61" s="7"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B62" s="8" t="n">
+      <c r="A62" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B62" s="9" t="n">
         <v>0.5429</v>
       </c>
-      <c r="C62" s="9" t="n">
+      <c r="C62" s="21" t="n">
         <v>0.5164</v>
       </c>
-      <c r="D62" s="8" t="n">
+      <c r="D62" s="10" t="n">
         <v>0.5429</v>
       </c>
-      <c r="E62" s="8" t="n">
+      <c r="E62" s="10" t="n">
         <v>0.5378</v>
       </c>
-      <c r="F62" s="8"/>
-      <c r="G62" s="8"/>
-      <c r="H62" s="8" t="n">
+      <c r="F62" s="10"/>
+      <c r="G62" s="10"/>
+      <c r="H62" s="11" t="n">
         <v>0.7951</v>
       </c>
-      <c r="I62" s="9" t="n">
+      <c r="I62" s="10" t="n">
         <v>0.7567</v>
       </c>
-      <c r="J62" s="8" t="n">
+      <c r="J62" s="10" t="n">
         <v>0.791</v>
       </c>
-      <c r="K62" s="8" t="n">
+      <c r="K62" s="10" t="n">
         <v>0.7593</v>
       </c>
-      <c r="L62" s="10"/>
+      <c r="L62" s="12"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B66" s="4" t="n">
         <v>469.4764</v>
       </c>
-      <c r="C66" s="4" t="n">
+      <c r="C66" s="5" t="n">
         <v>467.7033</v>
       </c>
-      <c r="D66" s="5" t="n">
+      <c r="D66" s="19" t="n">
         <v>467.2</v>
       </c>
-      <c r="E66" s="4" t="n">
+      <c r="E66" s="5" t="n">
         <v>518.8579</v>
       </c>
-      <c r="F66" s="4"/>
-      <c r="G66" s="4"/>
-      <c r="H66" s="5" t="n">
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
+      <c r="H66" s="6" t="n">
         <v>18.7691</v>
       </c>
-      <c r="I66" s="4" t="n">
+      <c r="I66" s="5" t="n">
         <v>22.7863</v>
       </c>
-      <c r="J66" s="4" t="n">
+      <c r="J66" s="5" t="n">
         <v>19.2732</v>
       </c>
-      <c r="K66" s="4" t="n">
+      <c r="K66" s="5" t="n">
         <v>40.3739</v>
       </c>
-      <c r="L66" s="6"/>
+      <c r="L66" s="7"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B67" s="8" t="n">
+      <c r="A67" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B67" s="20" t="n">
         <v>0.2956</v>
       </c>
-      <c r="C67" s="9" t="n">
+      <c r="C67" s="10" t="n">
         <v>0.1954</v>
       </c>
-      <c r="D67" s="8" t="n">
+      <c r="D67" s="10" t="n">
         <v>0.2806</v>
       </c>
-      <c r="E67" s="8" t="n">
+      <c r="E67" s="10" t="n">
         <v>0.2434</v>
       </c>
-      <c r="F67" s="8"/>
-      <c r="G67" s="8"/>
-      <c r="H67" s="8" t="n">
+      <c r="F67" s="10"/>
+      <c r="G67" s="10"/>
+      <c r="H67" s="11" t="n">
         <v>0.9718</v>
       </c>
-      <c r="I67" s="8" t="n">
+      <c r="I67" s="10" t="n">
         <v>0.9608</v>
       </c>
-      <c r="J67" s="8" t="n">
+      <c r="J67" s="10" t="n">
         <v>0.9703</v>
       </c>
-      <c r="K67" s="9" t="n">
+      <c r="K67" s="10" t="n">
         <v>0.9411</v>
       </c>
-      <c r="L67" s="10"/>
+      <c r="L67" s="12"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Upotpunjeni datasetovi sa predikcionim vrednostima za trazene godine, tako da odgovaraju u opsegu 1990-2017
</commit_message>
<xml_diff>
--- a/Fill NaN values dataset.xlsx
+++ b/Fill NaN values dataset.xlsx
@@ -113,7 +113,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -141,11 +141,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -262,7 +257,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -339,19 +334,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -462,8 +445,8 @@
   </sheetPr>
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -555,7 +538,7 @@
         <v>253.048</v>
       </c>
       <c r="I6" s="6" t="n">
-        <v>194.1651</v>
+        <v>191.683</v>
       </c>
       <c r="J6" s="5" t="n">
         <v>252.7337</v>
@@ -587,7 +570,7 @@
         <v>0.6816</v>
       </c>
       <c r="I7" s="11" t="n">
-        <v>0.6669</v>
+        <v>0.6721</v>
       </c>
       <c r="J7" s="10" t="n">
         <v>0.6815</v>
@@ -668,7 +651,7 @@
       <c r="B16" s="4" t="n">
         <v>711.9993</v>
       </c>
-      <c r="C16" s="19" t="n">
+      <c r="C16" s="5" t="n">
         <v>593.2072</v>
       </c>
       <c r="D16" s="5" t="n">
@@ -683,7 +666,7 @@
         <v>250.8493</v>
       </c>
       <c r="I16" s="6" t="n">
-        <v>162.6384</v>
+        <v>153.6216</v>
       </c>
       <c r="J16" s="5" t="n">
         <v>250.8493</v>
@@ -697,7 +680,7 @@
       <c r="A17" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="20" t="n">
+      <c r="B17" s="9" t="n">
         <v>-0.1156</v>
       </c>
       <c r="C17" s="10" t="n">
@@ -715,7 +698,7 @@
         <v>0.6069</v>
       </c>
       <c r="I17" s="11" t="n">
-        <v>0.6325</v>
+        <v>0.6562</v>
       </c>
       <c r="J17" s="10" t="n">
         <v>0.6069</v>
@@ -796,7 +779,7 @@
       <c r="B26" s="4" t="n">
         <v>4.2175</v>
       </c>
-      <c r="C26" s="19" t="n">
+      <c r="C26" s="5" t="n">
         <v>4.2175</v>
       </c>
       <c r="D26" s="5" t="n">
@@ -828,7 +811,7 @@
       <c r="B27" s="9" t="n">
         <v>-2.1855</v>
       </c>
-      <c r="C27" s="21" t="n">
+      <c r="C27" s="10" t="n">
         <v>-2.1856</v>
       </c>
       <c r="D27" s="10" t="n">
@@ -860,7 +843,7 @@
       <c r="B31" s="4" t="n">
         <v>104.8095</v>
       </c>
-      <c r="C31" s="19" t="n">
+      <c r="C31" s="5" t="n">
         <v>104.8095</v>
       </c>
       <c r="D31" s="5" t="n">
@@ -892,7 +875,7 @@
       <c r="B32" s="9" t="n">
         <v>0.1571</v>
       </c>
-      <c r="C32" s="21" t="n">
+      <c r="C32" s="10" t="n">
         <v>0.1571</v>
       </c>
       <c r="D32" s="10" t="n">
@@ -924,7 +907,7 @@
       <c r="B36" s="4" t="n">
         <v>1.0184</v>
       </c>
-      <c r="C36" s="19" t="n">
+      <c r="C36" s="5" t="n">
         <v>1.0184</v>
       </c>
       <c r="D36" s="5" t="n">
@@ -956,7 +939,7 @@
       <c r="B37" s="9" t="n">
         <v>-0.2979</v>
       </c>
-      <c r="C37" s="21" t="n">
+      <c r="C37" s="10" t="n">
         <v>-0.2979</v>
       </c>
       <c r="D37" s="10" t="n">
@@ -1046,7 +1029,7 @@
       <c r="L42" s="12"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="22"/>
+      <c r="B45" s="19"/>
       <c r="F45" s="0" t="s">
         <v>22</v>
       </c>
@@ -1055,65 +1038,65 @@
       <c r="A46" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B46" s="23" t="n">
+      <c r="B46" s="20" t="n">
         <v>0.2096</v>
       </c>
-      <c r="C46" s="24" t="n">
+      <c r="C46" s="21" t="n">
         <v>0.2096</v>
       </c>
-      <c r="D46" s="24" t="n">
+      <c r="D46" s="21" t="n">
         <v>0.2096</v>
       </c>
-      <c r="E46" s="24" t="n">
+      <c r="E46" s="21" t="n">
         <v>0.2096</v>
       </c>
-      <c r="F46" s="24"/>
-      <c r="G46" s="24"/>
-      <c r="H46" s="24" t="n">
+      <c r="F46" s="21"/>
+      <c r="G46" s="21"/>
+      <c r="H46" s="21" t="n">
         <v>0.2213</v>
       </c>
-      <c r="I46" s="24" t="n">
+      <c r="I46" s="21" t="n">
         <v>0.2213</v>
       </c>
-      <c r="J46" s="24" t="n">
+      <c r="J46" s="21" t="n">
         <v>0.2213</v>
       </c>
-      <c r="K46" s="24" t="n">
+      <c r="K46" s="21" t="n">
         <v>0.2213</v>
       </c>
-      <c r="L46" s="25"/>
+      <c r="L46" s="22"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B47" s="26" t="n">
+      <c r="B47" s="23" t="n">
         <v>0.1611</v>
       </c>
-      <c r="C47" s="27" t="n">
+      <c r="C47" s="24" t="n">
         <v>0.1611</v>
       </c>
-      <c r="D47" s="27" t="n">
+      <c r="D47" s="24" t="n">
         <v>0.1611</v>
       </c>
-      <c r="E47" s="27" t="n">
+      <c r="E47" s="24" t="n">
         <v>0.1611</v>
       </c>
-      <c r="F47" s="27"/>
-      <c r="G47" s="27"/>
-      <c r="H47" s="27" t="n">
+      <c r="F47" s="24"/>
+      <c r="G47" s="24"/>
+      <c r="H47" s="24" t="n">
         <v>0.1142</v>
       </c>
-      <c r="I47" s="27" t="n">
+      <c r="I47" s="24" t="n">
         <v>0.1142</v>
       </c>
-      <c r="J47" s="27" t="n">
+      <c r="J47" s="24" t="n">
         <v>0.1142</v>
       </c>
-      <c r="K47" s="27" t="n">
+      <c r="K47" s="24" t="n">
         <v>0.1142</v>
       </c>
-      <c r="L47" s="28"/>
+      <c r="L47" s="25"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="s">
@@ -1122,7 +1105,7 @@
       <c r="B51" s="4" t="n">
         <v>0.0382</v>
       </c>
-      <c r="C51" s="19" t="n">
+      <c r="C51" s="5" t="n">
         <v>0.0358</v>
       </c>
       <c r="D51" s="5" t="n">
@@ -1139,7 +1122,7 @@
       <c r="I51" s="5" t="n">
         <v>0.011</v>
       </c>
-      <c r="J51" s="19" t="n">
+      <c r="J51" s="5" t="n">
         <v>0.0102</v>
       </c>
       <c r="K51" s="5" t="n">
@@ -1148,13 +1131,13 @@
       <c r="L51" s="7"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="29" t="s">
+      <c r="A52" s="26" t="s">
         <v>24</v>
       </c>
       <c r="B52" s="9" t="n">
         <v>0.611</v>
       </c>
-      <c r="C52" s="21" t="n">
+      <c r="C52" s="10" t="n">
         <v>0.6004</v>
       </c>
       <c r="D52" s="10" t="n">
@@ -1171,7 +1154,7 @@
       <c r="I52" s="10" t="n">
         <v>0.8773</v>
       </c>
-      <c r="J52" s="21" t="n">
+      <c r="J52" s="10" t="n">
         <v>0.8955</v>
       </c>
       <c r="K52" s="10" t="n">
@@ -1186,7 +1169,7 @@
       <c r="B56" s="4" t="n">
         <v>0.0325</v>
       </c>
-      <c r="C56" s="19" t="n">
+      <c r="C56" s="5" t="n">
         <v>0.0295</v>
       </c>
       <c r="D56" s="5" t="n">
@@ -1218,7 +1201,7 @@
       <c r="B57" s="9" t="n">
         <v>0.6079</v>
       </c>
-      <c r="C57" s="21" t="n">
+      <c r="C57" s="10" t="n">
         <v>0.6</v>
       </c>
       <c r="D57" s="10" t="n">
@@ -1250,7 +1233,7 @@
       <c r="B61" s="4" t="n">
         <v>0.0295</v>
       </c>
-      <c r="C61" s="19" t="n">
+      <c r="C61" s="5" t="n">
         <v>0.0275</v>
       </c>
       <c r="D61" s="5" t="n">
@@ -1276,13 +1259,13 @@
       <c r="L61" s="7"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="29" t="s">
+      <c r="A62" s="26" t="s">
         <v>26</v>
       </c>
       <c r="B62" s="9" t="n">
         <v>0.5429</v>
       </c>
-      <c r="C62" s="21" t="n">
+      <c r="C62" s="10" t="n">
         <v>0.5164</v>
       </c>
       <c r="D62" s="10" t="n">
@@ -1317,7 +1300,7 @@
       <c r="C66" s="5" t="n">
         <v>467.7033</v>
       </c>
-      <c r="D66" s="19" t="n">
+      <c r="D66" s="5" t="n">
         <v>467.2</v>
       </c>
       <c r="E66" s="5" t="n">
@@ -1343,7 +1326,7 @@
       <c r="A67" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B67" s="20" t="n">
+      <c r="B67" s="9" t="n">
         <v>0.2956</v>
       </c>
       <c r="C67" s="10" t="n">

</xml_diff>

<commit_message>
fillovane nedostajuce vrednosti na dodatnim tabelama
</commit_message>
<xml_diff>
--- a/Fill NaN values dataset.xlsx
+++ b/Fill NaN values dataset.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="41">
   <si>
     <t xml:space="preserve">X Boost Regression (XBR)</t>
   </si>
@@ -104,6 +104,45 @@
   </si>
   <si>
     <t xml:space="preserve">FREEDOM OF PRESS DATA, TOTAL SCORE AS PREDICTING VALUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMPLOYERS PERCENTAGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INFLATION DATA SET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POPULATION DENSITY DATA SET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PTS-2019 DATA SET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNEPLOYMENT DATA SET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">URBAN POPULATION DATA SET </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCHOOLING DATA SET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCHOOLING DATA SET </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INTERNET USERS DATA SET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">global_state_of_democracy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ima mnogo kolona, pa se nece prikazivati rezultati ovde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCHOOL ENROLLMENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MILITARY EXPENDITURE</t>
   </si>
 </sst>
 </file>
@@ -113,7 +152,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -141,6 +180,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -257,7 +301,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -363,6 +407,22 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -443,10 +503,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L67"/>
+  <dimension ref="A1:L127"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A133" activeCellId="0" sqref="A133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1354,6 +1414,438 @@
       </c>
       <c r="L67" s="12"/>
     </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B71" s="5"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="5"/>
+      <c r="F71" s="5"/>
+      <c r="G71" s="5"/>
+      <c r="H71" s="6" t="n">
+        <v>2.14836</v>
+      </c>
+      <c r="I71" s="5"/>
+      <c r="J71" s="5"/>
+      <c r="K71" s="5"/>
+      <c r="L71" s="7"/>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B72" s="10"/>
+      <c r="C72" s="10"/>
+      <c r="D72" s="10"/>
+      <c r="E72" s="10"/>
+      <c r="F72" s="10"/>
+      <c r="G72" s="10"/>
+      <c r="H72" s="11" t="n">
+        <v>0.5374</v>
+      </c>
+      <c r="I72" s="10"/>
+      <c r="J72" s="10"/>
+      <c r="K72" s="10"/>
+      <c r="L72" s="12"/>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B76" s="5"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5"/>
+      <c r="E76" s="5"/>
+      <c r="F76" s="5"/>
+      <c r="G76" s="5"/>
+      <c r="H76" s="6" t="n">
+        <v>10478.9376</v>
+      </c>
+      <c r="I76" s="5"/>
+      <c r="J76" s="5"/>
+      <c r="K76" s="5"/>
+      <c r="L76" s="7"/>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B77" s="10"/>
+      <c r="C77" s="10"/>
+      <c r="D77" s="10"/>
+      <c r="E77" s="10"/>
+      <c r="F77" s="10"/>
+      <c r="G77" s="10"/>
+      <c r="H77" s="11" t="n">
+        <v>-0.0404</v>
+      </c>
+      <c r="I77" s="10"/>
+      <c r="J77" s="10"/>
+      <c r="K77" s="10"/>
+      <c r="L77" s="12"/>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B81" s="5"/>
+      <c r="C81" s="5"/>
+      <c r="D81" s="5"/>
+      <c r="E81" s="5"/>
+      <c r="F81" s="5"/>
+      <c r="G81" s="5"/>
+      <c r="H81" s="6" t="n">
+        <v>903214.712</v>
+      </c>
+      <c r="I81" s="5"/>
+      <c r="J81" s="5"/>
+      <c r="K81" s="5"/>
+      <c r="L81" s="7"/>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B82" s="10"/>
+      <c r="C82" s="10"/>
+      <c r="D82" s="10"/>
+      <c r="E82" s="10"/>
+      <c r="F82" s="10"/>
+      <c r="G82" s="10"/>
+      <c r="H82" s="11" t="n">
+        <v>0.719</v>
+      </c>
+      <c r="I82" s="10"/>
+      <c r="J82" s="10"/>
+      <c r="K82" s="10"/>
+      <c r="L82" s="12"/>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B86" s="5"/>
+      <c r="C86" s="5"/>
+      <c r="D86" s="5"/>
+      <c r="E86" s="5"/>
+      <c r="F86" s="5"/>
+      <c r="G86" s="5"/>
+      <c r="H86" s="6" t="n">
+        <v>1.0421</v>
+      </c>
+      <c r="I86" s="5"/>
+      <c r="J86" s="5"/>
+      <c r="K86" s="5"/>
+      <c r="L86" s="7"/>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B87" s="10"/>
+      <c r="C87" s="10"/>
+      <c r="D87" s="10"/>
+      <c r="E87" s="10"/>
+      <c r="F87" s="10"/>
+      <c r="G87" s="10"/>
+      <c r="H87" s="11" t="n">
+        <v>0.1344</v>
+      </c>
+      <c r="I87" s="10"/>
+      <c r="J87" s="10"/>
+      <c r="K87" s="10"/>
+      <c r="L87" s="12"/>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B91" s="5"/>
+      <c r="C91" s="5"/>
+      <c r="D91" s="5"/>
+      <c r="E91" s="5"/>
+      <c r="F91" s="5"/>
+      <c r="G91" s="5"/>
+      <c r="H91" s="6" t="n">
+        <v>8.4513</v>
+      </c>
+      <c r="I91" s="5"/>
+      <c r="J91" s="5"/>
+      <c r="K91" s="5"/>
+      <c r="L91" s="7"/>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B92" s="10"/>
+      <c r="C92" s="10"/>
+      <c r="D92" s="10"/>
+      <c r="E92" s="10"/>
+      <c r="F92" s="10"/>
+      <c r="G92" s="10"/>
+      <c r="H92" s="11" t="n">
+        <v>0.0878</v>
+      </c>
+      <c r="I92" s="10"/>
+      <c r="J92" s="10"/>
+      <c r="K92" s="10"/>
+      <c r="L92" s="12"/>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B96" s="5"/>
+      <c r="C96" s="5"/>
+      <c r="D96" s="5"/>
+      <c r="E96" s="5"/>
+      <c r="F96" s="5"/>
+      <c r="G96" s="5"/>
+      <c r="H96" s="6" t="n">
+        <v>18.5049</v>
+      </c>
+      <c r="I96" s="5"/>
+      <c r="J96" s="5"/>
+      <c r="K96" s="5"/>
+      <c r="L96" s="7"/>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B97" s="10"/>
+      <c r="C97" s="10"/>
+      <c r="D97" s="10"/>
+      <c r="E97" s="10"/>
+      <c r="F97" s="10"/>
+      <c r="G97" s="10"/>
+      <c r="H97" s="11" t="n">
+        <v>0.0789</v>
+      </c>
+      <c r="I97" s="10"/>
+      <c r="J97" s="10"/>
+      <c r="K97" s="10"/>
+      <c r="L97" s="12"/>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B101" s="5"/>
+      <c r="C101" s="5"/>
+      <c r="D101" s="5"/>
+      <c r="E101" s="5"/>
+      <c r="F101" s="5"/>
+      <c r="G101" s="5"/>
+      <c r="H101" s="6" t="n">
+        <v>221.5145</v>
+      </c>
+      <c r="I101" s="5"/>
+      <c r="J101" s="5"/>
+      <c r="K101" s="5"/>
+      <c r="L101" s="7"/>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B102" s="10"/>
+      <c r="C102" s="10"/>
+      <c r="D102" s="10"/>
+      <c r="E102" s="10"/>
+      <c r="F102" s="10"/>
+      <c r="G102" s="10"/>
+      <c r="H102" s="11" t="n">
+        <v>0.3793</v>
+      </c>
+      <c r="I102" s="10"/>
+      <c r="J102" s="10"/>
+      <c r="K102" s="10"/>
+      <c r="L102" s="12"/>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B106" s="5"/>
+      <c r="C106" s="5"/>
+      <c r="D106" s="5"/>
+      <c r="E106" s="5"/>
+      <c r="F106" s="5"/>
+      <c r="G106" s="5"/>
+      <c r="H106" s="6" t="n">
+        <v>992.6983</v>
+      </c>
+      <c r="I106" s="5"/>
+      <c r="J106" s="5"/>
+      <c r="K106" s="5"/>
+      <c r="L106" s="7"/>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B107" s="10"/>
+      <c r="C107" s="10"/>
+      <c r="D107" s="10"/>
+      <c r="E107" s="10"/>
+      <c r="F107" s="10"/>
+      <c r="G107" s="10"/>
+      <c r="H107" s="11" t="n">
+        <v>0.3715</v>
+      </c>
+      <c r="I107" s="10"/>
+      <c r="J107" s="10"/>
+      <c r="K107" s="10"/>
+      <c r="L107" s="12"/>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B111" s="5"/>
+      <c r="C111" s="5"/>
+      <c r="D111" s="5"/>
+      <c r="E111" s="5"/>
+      <c r="F111" s="5"/>
+      <c r="G111" s="5"/>
+      <c r="H111" s="6" t="n">
+        <v>231.1542</v>
+      </c>
+      <c r="I111" s="5"/>
+      <c r="J111" s="5"/>
+      <c r="K111" s="5"/>
+      <c r="L111" s="7"/>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B112" s="10"/>
+      <c r="C112" s="10"/>
+      <c r="D112" s="10"/>
+      <c r="E112" s="10"/>
+      <c r="F112" s="10"/>
+      <c r="G112" s="10"/>
+      <c r="H112" s="11" t="n">
+        <v>0.4116</v>
+      </c>
+      <c r="I112" s="10"/>
+      <c r="J112" s="10"/>
+      <c r="K112" s="10"/>
+      <c r="L112" s="12"/>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C116" s="5"/>
+      <c r="D116" s="5"/>
+      <c r="E116" s="5"/>
+      <c r="F116" s="5"/>
+      <c r="G116" s="5"/>
+      <c r="H116" s="5"/>
+      <c r="I116" s="5"/>
+      <c r="J116" s="5"/>
+      <c r="K116" s="5"/>
+      <c r="L116" s="7"/>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B117" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="C117" s="10"/>
+      <c r="D117" s="10"/>
+      <c r="E117" s="10"/>
+      <c r="F117" s="10"/>
+      <c r="G117" s="10"/>
+      <c r="H117" s="10"/>
+      <c r="I117" s="10"/>
+      <c r="J117" s="10"/>
+      <c r="K117" s="10"/>
+      <c r="L117" s="12"/>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B121" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="C121" s="5"/>
+      <c r="D121" s="5"/>
+      <c r="E121" s="5"/>
+      <c r="F121" s="5"/>
+      <c r="G121" s="5"/>
+      <c r="H121" s="5"/>
+      <c r="I121" s="5"/>
+      <c r="J121" s="5"/>
+      <c r="K121" s="5"/>
+      <c r="L121" s="7"/>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B122" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="C122" s="10"/>
+      <c r="D122" s="10"/>
+      <c r="E122" s="10"/>
+      <c r="F122" s="10"/>
+      <c r="G122" s="10"/>
+      <c r="H122" s="10"/>
+      <c r="I122" s="10"/>
+      <c r="J122" s="10"/>
+      <c r="K122" s="10"/>
+      <c r="L122" s="12"/>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B126" s="5"/>
+      <c r="C126" s="5"/>
+      <c r="D126" s="5"/>
+      <c r="E126" s="5"/>
+      <c r="F126" s="5"/>
+      <c r="G126" s="5"/>
+      <c r="H126" s="6" t="n">
+        <v>15.981</v>
+      </c>
+      <c r="I126" s="5"/>
+      <c r="J126" s="5"/>
+      <c r="K126" s="5"/>
+      <c r="L126" s="7"/>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B127" s="10"/>
+      <c r="C127" s="10"/>
+      <c r="D127" s="10"/>
+      <c r="E127" s="10"/>
+      <c r="F127" s="10"/>
+      <c r="G127" s="10"/>
+      <c r="H127" s="11" t="n">
+        <v>0.0858</v>
+      </c>
+      <c r="I127" s="10"/>
+      <c r="J127" s="10"/>
+      <c r="K127" s="10"/>
+      <c r="L127" s="12"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Nova iteracija regresije tabela, izmenjen python kod, dodate nove informaciej za novu tabelu koja je uzeta u obzir i ubacene tabele za regresiju Borisu u folderu josTrebaRegresija/novo/novo2
</commit_message>
<xml_diff>
--- a/Fill NaN values dataset.xlsx
+++ b/Fill NaN values dataset.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="42">
   <si>
     <t xml:space="preserve">X Boost Regression (XBR)</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t xml:space="preserve">MILITARY EXPENDITURE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Human-rights-scores</t>
   </si>
 </sst>
 </file>
@@ -152,7 +155,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -180,11 +183,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -301,7 +299,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -414,15 +412,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -503,10 +497,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L127"/>
+  <dimension ref="A1:L132"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A133" activeCellId="0" sqref="A133"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G130" activeCellId="0" sqref="G130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1793,7 +1787,7 @@
       <c r="L121" s="7"/>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="30" t="s">
+      <c r="A122" s="8" t="s">
         <v>39</v>
       </c>
       <c r="B122" s="28" t="s">
@@ -1846,6 +1840,42 @@
       <c r="K127" s="10"/>
       <c r="L127" s="12"/>
     </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B131" s="5"/>
+      <c r="C131" s="5"/>
+      <c r="D131" s="5"/>
+      <c r="E131" s="5"/>
+      <c r="F131" s="5"/>
+      <c r="G131" s="5"/>
+      <c r="H131" s="6" t="n">
+        <v>1.5379</v>
+      </c>
+      <c r="I131" s="5"/>
+      <c r="J131" s="5"/>
+      <c r="K131" s="5"/>
+      <c r="L131" s="7"/>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B132" s="10"/>
+      <c r="C132" s="10"/>
+      <c r="D132" s="10"/>
+      <c r="E132" s="10"/>
+      <c r="F132" s="10"/>
+      <c r="G132" s="10"/>
+      <c r="H132" s="11" t="n">
+        <v>0.3864</v>
+      </c>
+      <c r="I132" s="10"/>
+      <c r="J132" s="10"/>
+      <c r="K132" s="10"/>
+      <c r="L132" s="12"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>